<commit_message>
Actualiza SOP templates y rutas
</commit_message>
<xml_diff>
--- a/imports/Elemento.xlsx
+++ b/imports/Elemento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Limpieza\LIMPIEZA_APP\sop_lavado_app\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CBF7A2-F48A-4BE6-8CF2-6534553EA997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCDCE4A-461A-4902-8692-F597C8E65065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elemento" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="294">
   <si>
     <t>EL</t>
   </si>
@@ -897,6 +897,21 @@
   </si>
   <si>
     <t>Direccion Oficina 002</t>
+  </si>
+  <si>
+    <t>Extintor</t>
+  </si>
+  <si>
+    <t>Tapete Decorativo</t>
+  </si>
+  <si>
+    <t>Silla Ejecutiva</t>
+  </si>
+  <si>
+    <t>Silla Tela</t>
+  </si>
+  <si>
+    <t>Archivero</t>
   </si>
 </sst>
 </file>
@@ -1163,20 +1178,6 @@
   </cellStyles>
   <dxfs count="74">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
@@ -1212,6 +1213,20 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2000,9 +2015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView zoomScale="61" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3524,7 +3539,9 @@
       <c r="E42" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F42" s="10"/>
+      <c r="F42" s="10" t="s">
+        <v>260</v>
+      </c>
       <c r="G42" s="10" t="s">
         <v>0</v>
       </c>
@@ -3554,7 +3571,9 @@
       <c r="E43" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F43" s="10"/>
+      <c r="F43" s="10" t="s">
+        <v>289</v>
+      </c>
       <c r="G43" s="10" t="s">
         <v>0</v>
       </c>
@@ -3584,7 +3603,9 @@
       <c r="E44" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F44" s="10"/>
+      <c r="F44" s="10" t="s">
+        <v>290</v>
+      </c>
       <c r="G44" s="10" t="s">
         <v>0</v>
       </c>
@@ -3614,7 +3635,9 @@
       <c r="E45" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="10"/>
+      <c r="F45" s="10" t="s">
+        <v>241</v>
+      </c>
       <c r="G45" s="10" t="s">
         <v>0</v>
       </c>
@@ -3644,7 +3667,9 @@
       <c r="E46" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="10"/>
+      <c r="F46" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="G46" s="10" t="s">
         <v>0</v>
       </c>
@@ -3674,7 +3699,9 @@
       <c r="E47" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F47" s="10"/>
+      <c r="F47" s="10" t="s">
+        <v>291</v>
+      </c>
       <c r="G47" s="10" t="s">
         <v>0</v>
       </c>
@@ -3704,7 +3731,9 @@
       <c r="E48" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F48" s="10"/>
+      <c r="F48" s="10" t="s">
+        <v>293</v>
+      </c>
       <c r="G48" s="10" t="s">
         <v>0</v>
       </c>
@@ -3734,7 +3763,9 @@
       <c r="E49" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F49" s="10"/>
+      <c r="F49" s="10" t="s">
+        <v>127</v>
+      </c>
       <c r="G49" s="10" t="s">
         <v>0</v>
       </c>
@@ -3764,7 +3795,9 @@
       <c r="E50" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F50" s="10"/>
+      <c r="F50" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="G50" s="10" t="s">
         <v>0</v>
       </c>
@@ -3807,7 +3840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" workbookViewId="0">
+    <sheetView zoomScale="70" workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
@@ -7015,24 +7048,24 @@
     <cfRule type="duplicateValues" dxfId="65" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:B36">
-    <cfRule type="duplicateValues" dxfId="64" priority="61"/>
-    <cfRule type="duplicateValues" dxfId="63" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
     <cfRule type="duplicateValues" dxfId="62" priority="60"/>
     <cfRule type="duplicateValues" dxfId="61" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:B40">
-    <cfRule type="duplicateValues" dxfId="60" priority="36"/>
-    <cfRule type="duplicateValues" dxfId="59" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
     <cfRule type="duplicateValues" dxfId="58" priority="56"/>
     <cfRule type="duplicateValues" dxfId="57" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="duplicateValues" dxfId="56" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="55" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
     <cfRule type="duplicateValues" dxfId="54" priority="50"/>
@@ -7051,28 +7084,28 @@
     <cfRule type="duplicateValues" dxfId="47" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="46" priority="42"/>
-    <cfRule type="duplicateValues" dxfId="45" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="43" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
     <cfRule type="duplicateValues" dxfId="42" priority="39"/>
     <cfRule type="duplicateValues" dxfId="41" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="duplicateValues" dxfId="40" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="duplicateValues" dxfId="38" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="37" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="duplicateValues" dxfId="36" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
     <cfRule type="duplicateValues" dxfId="34" priority="29"/>
@@ -7091,56 +7124,56 @@
     <cfRule type="duplicateValues" dxfId="27" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60:B61">
-    <cfRule type="duplicateValues" dxfId="26" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="duplicateValues" dxfId="24" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="duplicateValues" dxfId="20" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="duplicateValues" dxfId="18" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68:B69">
-    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70:B71">
-    <cfRule type="duplicateValues" dxfId="12" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
     <cfRule type="duplicateValues" dxfId="10" priority="4"/>
     <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B73">
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P3:P8 P10">
-    <cfRule type="duplicateValues" dxfId="8" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="duplicateValues" dxfId="7" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="duplicateValues" dxfId="6" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S30">
-    <cfRule type="duplicateValues" dxfId="5" priority="76"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B73">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="76"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7152,7 +7185,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7699,13 +7732,13 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="O3:O8 O10">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios BD Nuevas Areas + Consecuentes
</commit_message>
<xml_diff>
--- a/imports/Elemento.xlsx
+++ b/imports/Elemento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Limpieza\LIMPIEZA_APP\sop_lavado_app\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD50905F-762B-4267-94FB-D297CC4063FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25C0FB4-DF00-4EF3-A91E-6C32398CFC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3242" uniqueCount="585">
   <si>
     <t>EL</t>
   </si>
@@ -1656,6 +1656,135 @@
   </si>
   <si>
     <t>EL-CH-015</t>
+  </si>
+  <si>
+    <t>EL-LM-022</t>
+  </si>
+  <si>
+    <t>PD-IN-CO-001</t>
+  </si>
+  <si>
+    <t>EL-BO-015</t>
+  </si>
+  <si>
+    <t>EL-BP-018</t>
+  </si>
+  <si>
+    <t>VIGAS</t>
+  </si>
+  <si>
+    <t>VG</t>
+  </si>
+  <si>
+    <t>EL-VG-001</t>
+  </si>
+  <si>
+    <t>VIGA</t>
+  </si>
+  <si>
+    <t>Viga Techo</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>TUBERIA</t>
+  </si>
+  <si>
+    <t>Tuberia Techo</t>
+  </si>
+  <si>
+    <t>EL-TU-001</t>
+  </si>
+  <si>
+    <t>EL-AH-022</t>
+  </si>
+  <si>
+    <t>Mueble Medicamentos</t>
+  </si>
+  <si>
+    <t>EL-MU-005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesa Pasteur </t>
+  </si>
+  <si>
+    <t>EL-ME-004</t>
+  </si>
+  <si>
+    <t>Mesa Movil</t>
+  </si>
+  <si>
+    <t>EL-ME-005</t>
+  </si>
+  <si>
+    <t>EL-EC-012</t>
+  </si>
+  <si>
+    <t>EL-SI-015</t>
+  </si>
+  <si>
+    <t>EL-SI-016</t>
+  </si>
+  <si>
+    <t>Silla Madera</t>
+  </si>
+  <si>
+    <t>CAMILLA</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>EL-CA-001</t>
+  </si>
+  <si>
+    <t>Camilla</t>
+  </si>
+  <si>
+    <t>BANQUILLO</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>EL-BN-001</t>
+  </si>
+  <si>
+    <t>Banquillo</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>BASCULA</t>
+  </si>
+  <si>
+    <t>EL-BC-001</t>
+  </si>
+  <si>
+    <t>Bascula</t>
+  </si>
+  <si>
+    <t>EL-LM-023</t>
+  </si>
+  <si>
+    <t>Lampara Examen</t>
+  </si>
+  <si>
+    <t>EL-AR-007</t>
+  </si>
+  <si>
+    <t>Ventilador</t>
+  </si>
+  <si>
+    <t>EL-LZ-018</t>
+  </si>
+  <si>
+    <t>EL-PU-018</t>
+  </si>
+  <si>
+    <t>EL-CH-018</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1981,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1972,11 +2101,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="143">
+  <dxfs count="152">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2003,6 +2138,11 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2522,11 +2662,44 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2539,6 +2712,18 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2708,11 +2893,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -3206,8 +3386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P311"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C243" sqref="C243"/>
+    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="66" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J244" sqref="J244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3216,8 +3396,8 @@
     <col min="2" max="2" width="15.73046875" customWidth="1"/>
     <col min="3" max="3" width="15" style="6" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="17.265625" customWidth="1"/>
-    <col min="8" max="8" width="15.3984375" customWidth="1"/>
+    <col min="6" max="6" width="21.73046875" customWidth="1"/>
+    <col min="8" max="8" width="14.265625" customWidth="1"/>
     <col min="9" max="9" width="12.3984375" customWidth="1"/>
     <col min="10" max="10" width="27.86328125" customWidth="1"/>
     <col min="11" max="11" width="6.46484375" customWidth="1"/>
@@ -4595,8 +4775,12 @@
       <c r="J36" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="L36" s="15"/>
-      <c r="M36" s="14"/>
+      <c r="L36" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
@@ -4629,6 +4813,12 @@
       <c r="J37" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="L37" s="42" t="s">
+        <v>552</v>
+      </c>
+      <c r="M37" s="41" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="38" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
@@ -4661,6 +4851,12 @@
       <c r="J38" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="L38" s="42" t="s">
+        <v>566</v>
+      </c>
+      <c r="M38" s="41" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="39" spans="1:13" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
@@ -4693,6 +4889,12 @@
       <c r="J39" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="L39" s="42" t="s">
+        <v>570</v>
+      </c>
+      <c r="M39" s="41" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="40" spans="1:13" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
@@ -4725,6 +4927,12 @@
       <c r="J40" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="L40" s="42" t="s">
+        <v>575</v>
+      </c>
+      <c r="M40" s="41" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
@@ -11200,39 +11408,419 @@
         <v>152</v>
       </c>
     </row>
-    <row r="240" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="241" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="242" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="243" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="244" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="245" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="246" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="247" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="248" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="249" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="250" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="251" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="252" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="253" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="254" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="255" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="256" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="257" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="258" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="259" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="260" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="261" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="262" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="263" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="264" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="265" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="266" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="267" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="268" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="269" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="270" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="271" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="272" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="240" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A240" s="41" t="s">
+        <v>542</v>
+      </c>
+      <c r="B240" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D240" s="41">
+        <v>2</v>
+      </c>
+      <c r="E240" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A241" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B241" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D241" s="1">
+        <v>1</v>
+      </c>
+      <c r="E241" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F241" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A242" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B242" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D242" s="1">
+        <v>1</v>
+      </c>
+      <c r="E242" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A243" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B243" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D243" s="41">
+        <v>2</v>
+      </c>
+      <c r="E243" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A244" s="41" t="s">
+        <v>554</v>
+      </c>
+      <c r="B244" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C244" s="42" t="s">
+        <v>552</v>
+      </c>
+      <c r="D244" s="41">
+        <v>1</v>
+      </c>
+      <c r="E244" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F244" s="41" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A245" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B245" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D245" s="41">
+        <v>1</v>
+      </c>
+      <c r="E245" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F245" s="41" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A246" s="41" t="s">
+        <v>557</v>
+      </c>
+      <c r="B246" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D246" s="41">
+        <v>1</v>
+      </c>
+      <c r="E246" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F246" s="41" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A247" s="41" t="s">
+        <v>559</v>
+      </c>
+      <c r="B247" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D247" s="41">
+        <v>1</v>
+      </c>
+      <c r="E247" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F247" s="41" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A248" s="41" t="s">
+        <v>561</v>
+      </c>
+      <c r="B248" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D248" s="41">
+        <v>1</v>
+      </c>
+      <c r="E248" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F248" s="41" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A249" s="41" t="s">
+        <v>562</v>
+      </c>
+      <c r="B249" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C249" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D249" s="41">
+        <v>1</v>
+      </c>
+      <c r="E249" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F249" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A250" s="41" t="s">
+        <v>563</v>
+      </c>
+      <c r="B250" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D250" s="41">
+        <v>1</v>
+      </c>
+      <c r="E250" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F250" s="41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A251" s="41" t="s">
+        <v>564</v>
+      </c>
+      <c r="B251" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D251" s="41">
+        <v>2</v>
+      </c>
+      <c r="E251" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F251" s="41" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A252" s="41" t="s">
+        <v>568</v>
+      </c>
+      <c r="B252" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="D252" s="41">
+        <v>1</v>
+      </c>
+      <c r="E252" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F252" s="41" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A253" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="B253" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D253" s="1">
+        <v>1</v>
+      </c>
+      <c r="E253" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F253" s="41" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A254" s="41" t="s">
+        <v>576</v>
+      </c>
+      <c r="B254" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C254" s="42" t="s">
+        <v>575</v>
+      </c>
+      <c r="D254" s="41">
+        <v>1</v>
+      </c>
+      <c r="E254" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F254" s="41" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A255" s="41" t="s">
+        <v>578</v>
+      </c>
+      <c r="B255" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D255" s="41">
+        <v>1</v>
+      </c>
+      <c r="E255" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F255" s="41" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A256" s="41" t="s">
+        <v>580</v>
+      </c>
+      <c r="B256" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C256" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D256" s="41">
+        <v>1</v>
+      </c>
+      <c r="E256" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F256" s="9" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A257" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B257" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D257" s="41">
+        <v>1</v>
+      </c>
+      <c r="E257" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F257" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A258" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B258" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D258" s="41">
+        <v>1</v>
+      </c>
+      <c r="E258" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F258" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A259" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B259" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D259" s="41">
+        <v>1</v>
+      </c>
+      <c r="E259" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="261" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="262" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="263" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="264" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="265" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="266" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="267" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="268" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="269" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="270" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="271" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="272" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="273" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="274" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="275" ht="28.7" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -11282,179 +11870,204 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1:A2 A230:A1048576">
-    <cfRule type="duplicateValues" dxfId="142" priority="2016"/>
-    <cfRule type="duplicateValues" dxfId="141" priority="1611"/>
-    <cfRule type="duplicateValues" dxfId="140" priority="1591"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="1616"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="1636"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="2041"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A140 A142:A229">
-    <cfRule type="duplicateValues" dxfId="139" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A159">
-    <cfRule type="duplicateValues" dxfId="138" priority="67"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A284">
-    <cfRule type="duplicateValues" dxfId="137" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A141">
-    <cfRule type="duplicateValues" dxfId="136" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A161:A162">
-    <cfRule type="duplicateValues" dxfId="135" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A163">
-    <cfRule type="duplicateValues" dxfId="134" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A164:A165">
-    <cfRule type="duplicateValues" dxfId="133" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A166:A167">
-    <cfRule type="duplicateValues" dxfId="132" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A168:A169">
-    <cfRule type="duplicateValues" dxfId="131" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A170">
-    <cfRule type="duplicateValues" dxfId="130" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A171:A172">
-    <cfRule type="duplicateValues" dxfId="129" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A174:A175">
-    <cfRule type="duplicateValues" dxfId="128" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A188:A189">
-    <cfRule type="duplicateValues" dxfId="127" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A197:A198">
-    <cfRule type="duplicateValues" dxfId="126" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A207:A208">
-    <cfRule type="duplicateValues" dxfId="125" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A219">
-    <cfRule type="duplicateValues" dxfId="124" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A231">
-    <cfRule type="duplicateValues" dxfId="123" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A233">
-    <cfRule type="duplicateValues" dxfId="122" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="121" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A235">
-    <cfRule type="duplicateValues" dxfId="120" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A237">
-    <cfRule type="duplicateValues" dxfId="119" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A238">
-    <cfRule type="duplicateValues" dxfId="118" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239">
-    <cfRule type="duplicateValues" dxfId="117" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B174">
-    <cfRule type="duplicateValues" dxfId="116" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B188">
-    <cfRule type="duplicateValues" dxfId="115" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B189">
-    <cfRule type="duplicateValues" dxfId="114" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B197">
-    <cfRule type="duplicateValues" dxfId="113" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B198">
-    <cfRule type="duplicateValues" dxfId="112" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B228">
-    <cfRule type="duplicateValues" dxfId="111" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B229">
-    <cfRule type="duplicateValues" dxfId="110" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="duplicateValues" dxfId="109" priority="283"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="308"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="duplicateValues" dxfId="108" priority="282"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="307"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53 H40:H41 H43 H45:H47">
-    <cfRule type="duplicateValues" dxfId="107" priority="655"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="680"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60">
-    <cfRule type="duplicateValues" dxfId="106" priority="353"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="378"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="duplicateValues" dxfId="105" priority="348"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="373"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74:H75">
-    <cfRule type="duplicateValues" dxfId="104" priority="1271"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="1296"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="duplicateValues" dxfId="103" priority="268"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="293"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="duplicateValues" dxfId="102" priority="237"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="262"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90 H86">
-    <cfRule type="duplicateValues" dxfId="101" priority="1064"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="1089"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H91">
-    <cfRule type="duplicateValues" dxfId="100" priority="235"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="260"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92">
-    <cfRule type="duplicateValues" dxfId="99" priority="314"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="339"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H105">
-    <cfRule type="duplicateValues" dxfId="98" priority="184"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="209"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H108">
-    <cfRule type="duplicateValues" dxfId="97" priority="158"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="183"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H142">
-    <cfRule type="duplicateValues" dxfId="96" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H143">
-    <cfRule type="duplicateValues" dxfId="95" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H150">
-    <cfRule type="duplicateValues" dxfId="94" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H163">
-    <cfRule type="duplicateValues" dxfId="93" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H178">
-    <cfRule type="duplicateValues" dxfId="92" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H232">
-    <cfRule type="duplicateValues" dxfId="91" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L95:L123">
-    <cfRule type="duplicateValues" dxfId="90" priority="1668"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="1693"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:M40 L1:M2 M3:M36">
-    <cfRule type="duplicateValues" dxfId="89" priority="1175"/>
+  <conditionalFormatting sqref="L40:M40 L1:M2 M3:M39">
+    <cfRule type="duplicateValues" dxfId="99" priority="1200"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M29">
-    <cfRule type="duplicateValues" dxfId="88" priority="2005"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="2030"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M31">
-    <cfRule type="duplicateValues" dxfId="87" priority="2007"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="2032"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M36">
-    <cfRule type="duplicateValues" dxfId="86" priority="2009"/>
+  <conditionalFormatting sqref="M4:M39">
+    <cfRule type="duplicateValues" dxfId="96" priority="2034"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30:M31">
-    <cfRule type="duplicateValues" dxfId="85" priority="340"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="365"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="duplicateValues" dxfId="84" priority="339"/>
-    <cfRule type="duplicateValues" dxfId="83" priority="338"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="363"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="364"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P97:P128">
-    <cfRule type="duplicateValues" dxfId="82" priority="1670"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="1695"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A241">
+    <cfRule type="duplicateValues" dxfId="91" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A241">
+    <cfRule type="duplicateValues" dxfId="90" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A242">
+    <cfRule type="duplicateValues" dxfId="89" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A245">
+    <cfRule type="duplicateValues" dxfId="87" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C254">
+    <cfRule type="duplicateValues" dxfId="86" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A257">
+    <cfRule type="duplicateValues" dxfId="85" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A258">
+    <cfRule type="duplicateValues" dxfId="84" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A259">
+    <cfRule type="duplicateValues" dxfId="83" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A282">
+    <cfRule type="duplicateValues" dxfId="0" priority="2054"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14570,166 +15183,166 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B29">
+    <cfRule type="duplicateValues" dxfId="82" priority="88"/>
     <cfRule type="duplicateValues" dxfId="81" priority="89"/>
-    <cfRule type="duplicateValues" dxfId="80" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="79" priority="86"/>
-    <cfRule type="duplicateValues" dxfId="78" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="duplicateValues" dxfId="77" priority="84"/>
-    <cfRule type="duplicateValues" dxfId="76" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:B34">
+    <cfRule type="duplicateValues" dxfId="76" priority="82"/>
     <cfRule type="duplicateValues" dxfId="75" priority="83"/>
-    <cfRule type="duplicateValues" dxfId="74" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
+    <cfRule type="duplicateValues" dxfId="74" priority="80"/>
     <cfRule type="duplicateValues" dxfId="73" priority="81"/>
-    <cfRule type="duplicateValues" dxfId="72" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
+    <cfRule type="duplicateValues" dxfId="72" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="10"/>
     <cfRule type="duplicateValues" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="71" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="70" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="69" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="68" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="67" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="66" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="65" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
+    <cfRule type="duplicateValues" dxfId="65" priority="76"/>
     <cfRule type="duplicateValues" dxfId="64" priority="77"/>
-    <cfRule type="duplicateValues" dxfId="63" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
+    <cfRule type="duplicateValues" dxfId="63" priority="74"/>
     <cfRule type="duplicateValues" dxfId="62" priority="75"/>
-    <cfRule type="duplicateValues" dxfId="61" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
+    <cfRule type="duplicateValues" dxfId="61" priority="70"/>
     <cfRule type="duplicateValues" dxfId="60" priority="71"/>
-    <cfRule type="duplicateValues" dxfId="59" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
+    <cfRule type="duplicateValues" dxfId="59" priority="66"/>
     <cfRule type="duplicateValues" dxfId="58" priority="67"/>
-    <cfRule type="duplicateValues" dxfId="57" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="duplicateValues" dxfId="56" priority="64"/>
-    <cfRule type="duplicateValues" dxfId="55" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="duplicateValues" dxfId="54" priority="68"/>
-    <cfRule type="duplicateValues" dxfId="53" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
+    <cfRule type="duplicateValues" dxfId="53" priority="62"/>
     <cfRule type="duplicateValues" dxfId="52" priority="63"/>
-    <cfRule type="duplicateValues" dxfId="51" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
+    <cfRule type="duplicateValues" dxfId="51" priority="58"/>
     <cfRule type="duplicateValues" dxfId="50" priority="59"/>
-    <cfRule type="duplicateValues" dxfId="49" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
+    <cfRule type="duplicateValues" dxfId="49" priority="60"/>
     <cfRule type="duplicateValues" dxfId="48" priority="61"/>
-    <cfRule type="duplicateValues" dxfId="47" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="46" priority="54"/>
-    <cfRule type="duplicateValues" dxfId="45" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
+    <cfRule type="duplicateValues" dxfId="45" priority="52"/>
     <cfRule type="duplicateValues" dxfId="44" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="43" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
+    <cfRule type="duplicateValues" dxfId="43" priority="48"/>
     <cfRule type="duplicateValues" dxfId="42" priority="49"/>
-    <cfRule type="duplicateValues" dxfId="41" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
+    <cfRule type="duplicateValues" dxfId="41" priority="50"/>
     <cfRule type="duplicateValues" dxfId="40" priority="51"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
+    <cfRule type="duplicateValues" dxfId="39" priority="46"/>
     <cfRule type="duplicateValues" dxfId="38" priority="47"/>
-    <cfRule type="duplicateValues" dxfId="37" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="36" priority="44"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:B56">
+    <cfRule type="duplicateValues" dxfId="35" priority="42"/>
     <cfRule type="duplicateValues" dxfId="34" priority="43"/>
-    <cfRule type="duplicateValues" dxfId="33" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57:B58">
+    <cfRule type="duplicateValues" dxfId="33" priority="40"/>
     <cfRule type="duplicateValues" dxfId="32" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
+    <cfRule type="duplicateValues" dxfId="31" priority="38"/>
     <cfRule type="duplicateValues" dxfId="30" priority="39"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
+    <cfRule type="duplicateValues" dxfId="29" priority="36"/>
     <cfRule type="duplicateValues" dxfId="28" priority="37"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
+    <cfRule type="duplicateValues" dxfId="27" priority="32"/>
     <cfRule type="duplicateValues" dxfId="26" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="duplicateValues" dxfId="24" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
+    <cfRule type="duplicateValues" dxfId="23" priority="30"/>
     <cfRule type="duplicateValues" dxfId="22" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65:B66">
+    <cfRule type="duplicateValues" dxfId="21" priority="28"/>
     <cfRule type="duplicateValues" dxfId="20" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67:B68">
+    <cfRule type="duplicateValues" dxfId="19" priority="26"/>
     <cfRule type="duplicateValues" dxfId="18" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
+    <cfRule type="duplicateValues" dxfId="17" priority="24"/>
     <cfRule type="duplicateValues" dxfId="16" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
+    <cfRule type="duplicateValues" dxfId="15" priority="22"/>
     <cfRule type="duplicateValues" dxfId="14" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P8 P10">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1 S2:S34">
-    <cfRule type="duplicateValues" dxfId="9" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S28">
-    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S30">
-    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S34">
-    <cfRule type="duplicateValues" dxfId="6" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29:S30">
-    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
+    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
     <cfRule type="duplicateValues" dxfId="4" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15222,13 +15835,13 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="O3:O8 O10">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>